<commit_message>
renamed suggested auditories column
</commit_message>
<xml_diff>
--- a/data/VIDOMOST_DORUChEN_2 сем_ДВ_ДМ і ПТМ.xlsx
+++ b/data/VIDOMOST_DORUChEN_2 сем_ДВ_ДМ і ПТМ.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$I$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$K$56</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="63">
   <si>
     <t>МІНІСТЕРСТВО ОСВІТИ І НАУКИ УКРАЇНИ</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Аналіз умов експлуатації деталей машин та інструменту</t>
   </si>
   <si>
-    <t>Іф-217, Іф-218сп,              Іф-228сп, Іф-617</t>
-  </si>
-  <si>
     <t>Надійність технічних систем</t>
   </si>
   <si>
@@ -311,6 +308,94 @@
       </rPr>
       <t>Володимирович</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>І</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Ф</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-217, І</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Ф</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-218сп,              І</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Ф</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-228сп, І</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Ф</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-617</t>
+    </r>
+  </si>
+  <si>
+    <t>Пропозиції щодо аудиторій</t>
   </si>
 </sst>
 </file>
@@ -444,12 +529,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -480,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -549,6 +640,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -885,10 +994,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,48 +1008,50 @@
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
     <col min="6" max="7" width="12.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="8" max="9" width="27.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I1" s="11" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-    </row>
-    <row r="3" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.4">
-      <c r="A4" s="27" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.4">
+      <c r="A4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
@@ -950,21 +1061,23 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:13" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="1:14" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="13"/>
       <c r="C7" s="3"/>
@@ -973,22 +1086,24 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="I7" s="25"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-    </row>
-    <row r="9" spans="1:13" ht="11.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:14" ht="11.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="13"/>
       <c r="C9" s="3"/>
@@ -997,35 +1112,38 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="I9" s="25"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-    </row>
-    <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="14"/>
       <c r="C12" s="4"/>
@@ -1034,9 +1152,10 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="26"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
@@ -1062,10 +1181,13 @@
         <v>22</v>
       </c>
       <c r="I13" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -1093,8 +1215,11 @@
       <c r="I14" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1</v>
       </c>
@@ -1122,8 +1247,9 @@
       <c r="I15" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>2</v>
       </c>
@@ -1151,8 +1277,9 @@
       <c r="I16" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>3</v>
       </c>
@@ -1180,8 +1307,9 @@
       <c r="I17" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>4</v>
       </c>
@@ -1209,8 +1337,9 @@
       <c r="I18" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>5</v>
       </c>
@@ -1238,8 +1367,9 @@
       <c r="I19" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>6</v>
       </c>
@@ -1267,8 +1397,9 @@
       <c r="I20" s="18">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>7</v>
       </c>
@@ -1296,8 +1427,9 @@
       <c r="I21" s="18">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>8</v>
       </c>
@@ -1325,8 +1457,9 @@
       <c r="I22" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>9</v>
       </c>
@@ -1354,8 +1487,9 @@
       <c r="I23" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>10</v>
       </c>
@@ -1383,8 +1517,9 @@
       <c r="I24" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J24" s="28"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>11</v>
       </c>
@@ -1412,8 +1547,9 @@
       <c r="I25" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J25" s="28"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>12</v>
       </c>
@@ -1441,8 +1577,9 @@
       <c r="I26" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>13</v>
       </c>
@@ -1470,8 +1607,9 @@
       <c r="I27" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>14</v>
       </c>
@@ -1499,8 +1637,9 @@
       <c r="I28" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="27"/>
+    </row>
+    <row r="29" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>15</v>
       </c>
@@ -1528,8 +1667,9 @@
       <c r="I29" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="27"/>
+    </row>
+    <row r="30" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>16</v>
       </c>
@@ -1557,8 +1697,9 @@
       <c r="I30" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>17</v>
       </c>
@@ -1586,8 +1727,9 @@
       <c r="I31" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J31" s="28"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>18</v>
       </c>
@@ -1615,8 +1757,9 @@
       <c r="I32" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J32" s="27"/>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>19</v>
       </c>
@@ -1644,8 +1787,9 @@
       <c r="I33" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="27"/>
+    </row>
+    <row r="34" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>20</v>
       </c>
@@ -1673,8 +1817,9 @@
       <c r="I34" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="28"/>
+    </row>
+    <row r="35" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>21</v>
       </c>
@@ -1702,8 +1847,9 @@
       <c r="I35" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J35" s="28"/>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>22</v>
       </c>
@@ -1731,8 +1877,9 @@
       <c r="I36" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J36" s="28"/>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>23</v>
       </c>
@@ -1760,8 +1907,9 @@
       <c r="I37" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J37" s="28"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>24</v>
       </c>
@@ -1789,8 +1937,9 @@
       <c r="I38" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>25</v>
       </c>
@@ -1818,8 +1967,9 @@
       <c r="I39" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>26</v>
       </c>
@@ -1847,8 +1997,9 @@
       <c r="I40" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>27</v>
       </c>
@@ -1876,8 +2027,9 @@
       <c r="I41" s="24">
         <v>545</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>28</v>
       </c>
@@ -1905,8 +2057,9 @@
       <c r="I42" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J42" s="27"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>29</v>
       </c>
@@ -1934,8 +2087,9 @@
       <c r="I43" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J43" s="27"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>30</v>
       </c>
@@ -1963,8 +2117,9 @@
       <c r="I44" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>31</v>
       </c>
@@ -1992,8 +2147,9 @@
       <c r="I45" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J45" s="27"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>32</v>
       </c>
@@ -2021,8 +2177,9 @@
       <c r="I46" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J46" s="27"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>33</v>
       </c>
@@ -2030,7 +2187,7 @@
         <v>58</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D47" s="24" t="s">
         <v>42</v>
@@ -2050,8 +2207,9 @@
       <c r="I47" s="18">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>34</v>
       </c>
@@ -2059,7 +2217,7 @@
         <v>58</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>39</v>
@@ -2079,13 +2237,14 @@
       <c r="I48" s="18">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J48" s="27"/>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>35</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>45</v>
@@ -2103,18 +2262,19 @@
         <v>23</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I49" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="19">
         <v>36</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>45</v>
@@ -2132,52 +2292,56 @@
         <v>23</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I50" s="18">
         <v>545</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J50" s="27"/>
+    </row>
+    <row r="53" spans="1:10" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="17"/>
-      <c r="H53" s="32" t="s">
+      <c r="H53" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="32"/>
-    </row>
-    <row r="54" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H54" s="33" t="s">
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+    </row>
+    <row r="54" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I54" s="33"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="B11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="C28:C29">
     <cfRule type="uniqueValues" dxfId="1" priority="2"/>
@@ -2187,6 +2351,6 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="84" fitToHeight="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" fitToHeight="2" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>